<commit_message>
Good spanish classfication, updated scripts
</commit_message>
<xml_diff>
--- a/datasets/categories_2013-02-12/category_topic_resolver.xlsx
+++ b/datasets/categories_2013-02-12/category_topic_resolver.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="20140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Eng_Spa_Topics" sheetId="1" r:id="rId1"/>
@@ -289,8 +289,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -363,7 +447,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -397,6 +481,48 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +556,48 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1041,14 +1209,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.1640625" bestFit="1" customWidth="1"/>
@@ -1107,16 +1276,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -1130,16 +1299,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -1153,16 +1322,16 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -1175,14 +1344,17 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
         <v>2</v>
@@ -1196,13 +1368,16 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
         <v>4</v>
@@ -1216,16 +1391,16 @@
         <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J8" t="s">
         <v>66</v>
@@ -1238,14 +1413,17 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
@@ -1259,16 +1437,16 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
         <v>7</v>
@@ -1282,16 +1460,16 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
         <v>8</v>
@@ -1304,14 +1482,17 @@
       <c r="B12" t="s">
         <v>9</v>
       </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -1325,13 +1506,16 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
         <v>10</v>
@@ -1345,16 +1529,16 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
         <v>2</v>
@@ -1371,13 +1555,13 @@
         <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s">
         <v>7</v>
@@ -1391,16 +1575,16 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
@@ -1414,16 +1598,13 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="J17" t="s">
         <v>12</v>
@@ -1437,16 +1618,13 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="H18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
         <v>10</v>
@@ -1460,10 +1638,10 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="J19" t="s">
         <v>2</v>
@@ -1477,10 +1655,10 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J20" t="s">
         <v>2</v>
@@ -1494,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J21" t="s">
         <v>0</v>
@@ -1510,11 +1688,8 @@
       <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J22" t="s">
         <v>66</v>
@@ -1527,11 +1702,8 @@
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="J23" t="s">
         <v>13</v>
@@ -1545,7 +1717,7 @@
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>14</v>
@@ -1558,11 +1730,8 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" t="s">
         <v>10</v>
@@ -1635,6 +1804,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="G2:H18">
+    <sortCondition ref="G2:G18"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>